<commit_message>
xlsx: vertical loop support for more cases with formulas
</commit_message>
<xml_diff>
--- a/packages/jsreport-xlsx/test/xlsx/loop-update-formula-cells.xlsx
+++ b/packages/jsreport-xlsx/test/xlsx/loop-update-formula-cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/jsreport/jsreport/packages/jsreport-xlsx/test/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B8A904-3F4C-614A-AD97-486B5AD0B85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBDA684-169E-2842-9E6B-4706664EF707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2020" windowWidth="28040" windowHeight="17440" xr2:uid="{E64D1ECD-F10D-4745-832B-F27334D20F18}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="19200" windowHeight="10560" xr2:uid="{E64D1ECD-F10D-4745-832B-F27334D20F18}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -429,7 +428,7 @@
   <dimension ref="C2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>